<commit_message>
Agregando prefijo ks_ a las tablas
</commit_message>
<xml_diff>
--- a/recursos/Galenicum - Traslados Abril 2020 costeado.xlsx
+++ b/recursos/Galenicum - Traslados Abril 2020 costeado.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scc/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Dropbox\Rafael\Proyectos\Proyectos_Web\karius\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D09849-221D-F449-99D3-2F7DF63A250C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{80FC1E60-29B2-4476-A277-0807E2C6DFCC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Movilidades" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja3" sheetId="3" r:id="rId2"/>
-    <sheet name="Traslado personal" sheetId="2" r:id="rId3"/>
+    <sheet name="Traslado personal" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Movilidades!$A$8:$G$54</definedName>
@@ -242,9 +240,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -392,19 +390,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -430,6 +416,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -744,36 +742,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278CCE68-9B1D-42E2-BB2D-BA0515B7CFFE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:J58"/>
   <sheetViews>
-    <sheetView topLeftCell="B42" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="39.1640625" customWidth="1"/>
-    <col min="3" max="3" width="51.1640625" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="18.83203125" style="6" customWidth="1"/>
-    <col min="7" max="7" width="17.5" style="6" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" customWidth="1"/>
+    <col min="3" max="3" width="51.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="6" customWidth="1"/>
     <col min="8" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
@@ -783,12 +781,12 @@
       <c r="I5">
         <v>20</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="15">
         <f>I5/H5</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>12</v>
       </c>
@@ -811,8 +809,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43922</v>
       </c>
@@ -825,13 +823,13 @@
       <c r="D10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="20">
+      <c r="E10" s="16">
         <v>9.3333333333333321</v>
       </c>
-      <c r="F10" s="28">
-        <v>40</v>
-      </c>
-      <c r="G10" s="22">
+      <c r="F10" s="24">
+        <v>40</v>
+      </c>
+      <c r="G10" s="18">
         <f>E10+F10</f>
         <v>49.333333333333329</v>
       </c>
@@ -839,15 +837,15 @@
         <f>ROUND(E10/$J$5,0)</f>
         <v>28</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="16">
         <f>H10*$J$5</f>
         <v>9.3333333333333321</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="16">
         <v>9.3333333333333321</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>43922</v>
       </c>
@@ -860,13 +858,13 @@
       <c r="D11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="16">
         <v>80</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="24">
         <v>28</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="18">
         <f t="shared" ref="G11:G13" si="0">E11+F11</f>
         <v>108</v>
       </c>
@@ -874,15 +872,15 @@
         <f t="shared" ref="H11:H13" si="1">ROUND(E11/$J$5,0)</f>
         <v>240</v>
       </c>
-      <c r="I11" s="20">
-        <f t="shared" ref="I11:J13" si="2">H11*$J$5</f>
+      <c r="I11" s="16">
+        <f t="shared" ref="I11:I13" si="2">H11*$J$5</f>
         <v>80</v>
       </c>
-      <c r="J11" s="20">
+      <c r="J11" s="16">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>43924</v>
       </c>
@@ -895,13 +893,13 @@
       <c r="D12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="16">
         <v>34</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="24">
         <v>15</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="18">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
@@ -909,15 +907,15 @@
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
-      <c r="I12" s="20">
+      <c r="I12" s="16">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="J12" s="20">
+      <c r="J12" s="16">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>43924</v>
       </c>
@@ -930,13 +928,13 @@
       <c r="D13" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="20">
+      <c r="E13" s="16">
         <v>8.6666666666666661</v>
       </c>
-      <c r="F13" s="28">
+      <c r="F13" s="24">
         <v>15</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="18">
         <f t="shared" si="0"/>
         <v>23.666666666666664</v>
       </c>
@@ -944,44 +942,44 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="16">
         <f t="shared" si="2"/>
         <v>8.6666666666666661</v>
       </c>
-      <c r="J13" s="20">
+      <c r="J13" s="16">
         <v>8.6666666666666661</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
-      <c r="G14" s="23">
+      <c r="G14" s="19">
         <f>SUM(G10:G13)</f>
         <v>229.99999999999997</v>
       </c>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-    </row>
-    <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+    </row>
+    <row r="18" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>12</v>
       </c>
@@ -1003,14 +1001,14 @@
       <c r="G18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
-    </row>
-    <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+    </row>
+    <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>43928</v>
       </c>
@@ -1023,13 +1021,13 @@
       <c r="D20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E20" s="16">
         <v>19.333333333333332</v>
       </c>
-      <c r="F20" s="28">
+      <c r="F20" s="24">
         <v>10</v>
       </c>
-      <c r="G20" s="22">
+      <c r="G20" s="18">
         <f t="shared" ref="G20" si="3">E20+F20</f>
         <v>29.333333333333332</v>
       </c>
@@ -1037,29 +1035,29 @@
         <f t="shared" ref="H20" si="4">ROUND(E20/$J$5,0)</f>
         <v>58</v>
       </c>
-      <c r="I20" s="20">
-        <f t="shared" ref="I20:J20" si="5">H20*$J$5</f>
+      <c r="I20" s="16">
+        <f t="shared" ref="I20" si="5">H20*$J$5</f>
         <v>19.333333333333332</v>
       </c>
-      <c r="J20" s="20">
+      <c r="J20" s="16">
         <v>19.333333333333332</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
       <c r="D21" s="13"/>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
-      <c r="G21" s="22">
+      <c r="G21" s="18">
         <f>SUM(G20)</f>
         <v>29.333333333333332</v>
       </c>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -1067,25 +1065,25 @@
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="G22" s="9"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-    </row>
-    <row r="26" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+    </row>
+    <row r="26" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>12</v>
       </c>
@@ -1107,25 +1105,25 @@
       <c r="G26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I26" s="21"/>
-      <c r="J26" s="21"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
-      <c r="G28" s="22"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G28" s="18"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>43936</v>
       </c>
@@ -1136,29 +1134,29 @@
         <v>33</v>
       </c>
       <c r="D29" s="3"/>
-      <c r="E29" s="20">
-        <v>0</v>
-      </c>
-      <c r="F29" s="28">
+      <c r="E29" s="16">
+        <v>0</v>
+      </c>
+      <c r="F29" s="24">
         <v>22</v>
       </c>
-      <c r="G29" s="22">
-        <f t="shared" ref="G28:G33" si="6">E29+F29</f>
+      <c r="G29" s="18">
+        <f t="shared" ref="G29:G33" si="6">E29+F29</f>
         <v>22</v>
       </c>
       <c r="H29">
         <f t="shared" ref="H29:H33" si="7">ROUND(E29/$J$5,0)</f>
         <v>0</v>
       </c>
-      <c r="I29" s="20">
-        <f t="shared" ref="I29:J33" si="8">H29*$J$5</f>
-        <v>0</v>
-      </c>
-      <c r="J29" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I29" s="16">
+        <f t="shared" ref="I29:I33" si="8">H29*$J$5</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>43936</v>
       </c>
@@ -1171,13 +1169,13 @@
       <c r="D30" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E30" s="20">
+      <c r="E30" s="16">
         <v>6.6666666666666661</v>
       </c>
-      <c r="F30" s="28">
-        <v>40</v>
-      </c>
-      <c r="G30" s="22">
+      <c r="F30" s="24">
+        <v>40</v>
+      </c>
+      <c r="G30" s="18">
         <f t="shared" si="6"/>
         <v>46.666666666666664</v>
       </c>
@@ -1185,24 +1183,24 @@
         <f t="shared" si="7"/>
         <v>20</v>
       </c>
-      <c r="I30" s="20">
+      <c r="I30" s="16">
         <f t="shared" si="8"/>
         <v>6.6666666666666661</v>
       </c>
-      <c r="J30" s="20">
+      <c r="J30" s="16">
         <v>6.6666666666666661</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="20">
+      <c r="E31" s="16">
         <v>0</v>
       </c>
       <c r="F31" s="7"/>
-      <c r="G31" s="22">
+      <c r="G31" s="18">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
@@ -1210,15 +1208,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I31" s="20">
+      <c r="I31" s="16">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J31" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J31" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>43938</v>
       </c>
@@ -1229,13 +1227,13 @@
         <v>36</v>
       </c>
       <c r="D32" s="3"/>
-      <c r="E32" s="20">
-        <v>0</v>
-      </c>
-      <c r="F32" s="28">
-        <v>40</v>
-      </c>
-      <c r="G32" s="22">
+      <c r="E32" s="16">
+        <v>0</v>
+      </c>
+      <c r="F32" s="24">
+        <v>40</v>
+      </c>
+      <c r="G32" s="18">
         <f t="shared" si="6"/>
         <v>40</v>
       </c>
@@ -1243,15 +1241,15 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="I32" s="20">
+      <c r="I32" s="16">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="J32" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J32" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>43938</v>
       </c>
@@ -1264,13 +1262,13 @@
       <c r="D33" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E33" s="20">
+      <c r="E33" s="16">
         <v>79</v>
       </c>
-      <c r="F33" s="28">
+      <c r="F33" s="24">
         <v>25</v>
       </c>
-      <c r="G33" s="22">
+      <c r="G33" s="18">
         <f t="shared" si="6"/>
         <v>104</v>
       </c>
@@ -1278,42 +1276,42 @@
         <f t="shared" si="7"/>
         <v>237</v>
       </c>
-      <c r="I33" s="20">
+      <c r="I33" s="16">
         <f t="shared" si="8"/>
         <v>79</v>
       </c>
-      <c r="J33" s="20">
+      <c r="J33" s="16">
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G34" s="24">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G34" s="20">
         <f>SUM(G29:G33)</f>
         <v>212.66666666666666</v>
       </c>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-    </row>
-    <row r="39" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
+    </row>
+    <row r="39" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>12</v>
       </c>
@@ -1335,14 +1333,14 @@
       <c r="G39" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I39" s="21"/>
-      <c r="J39" s="21"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>43941</v>
       </c>
@@ -1355,13 +1353,13 @@
       <c r="D41" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E41" s="20">
+      <c r="E41" s="16">
         <v>36.666666666666664</v>
       </c>
-      <c r="F41" s="28">
+      <c r="F41" s="24">
         <v>17</v>
       </c>
-      <c r="G41" s="22">
+      <c r="G41" s="18">
         <f t="shared" ref="G41:G42" si="9">E41+F41</f>
         <v>53.666666666666664</v>
       </c>
@@ -1369,15 +1367,15 @@
         <f t="shared" ref="H41" si="10">ROUND(E41/$J$5,0)</f>
         <v>110</v>
       </c>
-      <c r="I41" s="20">
-        <f t="shared" ref="I41:J41" si="11">H41*$J$5</f>
+      <c r="I41" s="16">
+        <f t="shared" ref="I41" si="11">H41*$J$5</f>
         <v>36.666666666666664</v>
       </c>
-      <c r="J41" s="20">
+      <c r="J41" s="16">
         <v>36.666666666666664</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>43941</v>
       </c>
@@ -1389,46 +1387,46 @@
       </c>
       <c r="D42" s="3"/>
       <c r="E42" s="7"/>
-      <c r="F42" s="28">
+      <c r="F42" s="24">
         <v>19</v>
       </c>
-      <c r="G42" s="22">
+      <c r="G42" s="18">
         <f t="shared" si="9"/>
         <v>19</v>
       </c>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I42" s="16"/>
+      <c r="J42" s="16"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
-      <c r="G43" s="24">
+      <c r="G43" s="20">
         <f>SUM(G41:G42)</f>
         <v>72.666666666666657</v>
       </c>
-      <c r="J43" s="20"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J44" s="20"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J45" s="20"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J46" s="20"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J43" s="16"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J44" s="16"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J45" s="16"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J46" s="16"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="J47" s="20"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J48" s="20"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J49" s="20"/>
-    </row>
-    <row r="50" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J47" s="16"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J48" s="16"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J49" s="16"/>
+    </row>
+    <row r="50" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>12</v>
       </c>
@@ -1450,12 +1448,12 @@
       <c r="G50" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J50" s="21"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J51" s="20"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J50" s="17"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J51" s="16"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>43949</v>
       </c>
@@ -1468,10 +1466,10 @@
       <c r="D52" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="E52" s="20">
+      <c r="E52" s="16">
         <v>72</v>
       </c>
-      <c r="F52" s="28">
+      <c r="F52" s="24">
         <v>20</v>
       </c>
       <c r="G52" s="7">
@@ -1482,15 +1480,15 @@
         <f t="shared" ref="H52:H53" si="13">ROUND(E52/$J$5,0)</f>
         <v>216</v>
       </c>
-      <c r="I52" s="20">
-        <f t="shared" ref="I52:J53" si="14">H52*$J$5</f>
+      <c r="I52" s="16">
+        <f t="shared" ref="I52:I53" si="14">H52*$J$5</f>
         <v>72</v>
       </c>
-      <c r="J52" s="20">
+      <c r="J52" s="16">
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>43951</v>
       </c>
@@ -1503,10 +1501,10 @@
       <c r="D53" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E53" s="20">
+      <c r="E53" s="16">
         <v>25</v>
       </c>
-      <c r="F53" s="28">
+      <c r="F53" s="24">
         <v>10</v>
       </c>
       <c r="G53" s="7">
@@ -1517,49 +1515,49 @@
         <f t="shared" si="13"/>
         <v>75</v>
       </c>
-      <c r="I53" s="20">
+      <c r="I53" s="16">
         <f t="shared" si="14"/>
         <v>25</v>
       </c>
-      <c r="J53" s="20">
+      <c r="J53" s="16">
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="G54" s="6">
         <f>SUM(G52:G53)</f>
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F56" s="25" t="s">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F56" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="G56" s="26">
+      <c r="G56" s="22">
         <f>G14+G21+G34+G43+G54</f>
         <v>671.66666666666663</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F57" s="25" t="s">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F57" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="G57" s="26">
+      <c r="G57" s="22">
         <f>G56*18%</f>
         <v>120.89999999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="F58" s="25" t="s">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F58" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="G58" s="26">
+      <c r="G58" s="22">
         <f>G56+G57</f>
         <v>792.56666666666661</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A8:G54" xr:uid="{EE6B32A2-9CF9-124D-AC04-C9338B175666}"/>
+  <autoFilter ref="A8:G54"/>
   <mergeCells count="1">
     <mergeCell ref="A3:G3"/>
   </mergeCells>
@@ -1569,57 +1567,45 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{813D5FB3-07B6-DA46-8B3F-491760EDD9EA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5124C45-0479-4AC4-A871-5336322DC634}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" customWidth="1"/>
-    <col min="2" max="2" width="38.83203125" customWidth="1"/>
-    <col min="3" max="3" width="41" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-    <col min="5" max="6" width="16.5" customWidth="1"/>
-    <col min="7" max="7" width="30.83203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="38.85546875" customWidth="1"/>
+    <col min="3" max="3" width="48.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" style="6" customWidth="1"/>
     <col min="8" max="8" width="22" style="6" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="6"/>
+    <col min="9" max="9" width="10.85546875" style="6"/>
     <col min="10" max="11" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1632,7 +1618,7 @@
       <c r="D8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="28" t="s">
         <v>64</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -1645,10 +1631,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F9" s="18"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="29"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>43942</v>
       </c>
@@ -1667,13 +1653,13 @@
       <c r="F10" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="18">
         <v>8.35</v>
       </c>
-      <c r="H10" s="29">
-        <v>40</v>
-      </c>
-      <c r="I10" s="22">
+      <c r="H10" s="25">
+        <v>40</v>
+      </c>
+      <c r="I10" s="18">
         <f>E10+G10+H10</f>
         <v>141.70999999999998</v>
       </c>
@@ -1686,7 +1672,7 @@
         <v>25.052505250525051</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>43942</v>
       </c>
@@ -1699,11 +1685,11 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="29">
-        <v>40</v>
-      </c>
-      <c r="I11" s="22">
+      <c r="G11" s="18"/>
+      <c r="H11" s="25">
+        <v>40</v>
+      </c>
+      <c r="I11" s="18">
         <f>E11+G11+H11</f>
         <v>40</v>
       </c>
@@ -1716,7 +1702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>43943</v>
       </c>
@@ -1735,14 +1721,14 @@
       <c r="F12" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G12" s="22">
+      <c r="G12" s="18">
         <v>5.6779999999999999</v>
       </c>
-      <c r="H12" s="29">
-        <v>40</v>
-      </c>
-      <c r="I12" s="22">
-        <f t="shared" ref="I11:I20" si="2">E12+G12+H12</f>
+      <c r="H12" s="25">
+        <v>40</v>
+      </c>
+      <c r="I12" s="18">
+        <f t="shared" ref="I12:I19" si="2">E12+G12+H12</f>
         <v>134.02799999999999</v>
       </c>
       <c r="J12">
@@ -1754,7 +1740,7 @@
         <v>17.035703570357036</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>43943</v>
       </c>
@@ -1767,11 +1753,11 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="29">
-        <v>40</v>
-      </c>
-      <c r="I13" s="22">
+      <c r="G13" s="18"/>
+      <c r="H13" s="25">
+        <v>40</v>
+      </c>
+      <c r="I13" s="18">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
@@ -1784,7 +1770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>43945</v>
       </c>
@@ -1797,15 +1783,15 @@
       <c r="D14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="23">
         <v>82.671999999999997</v>
       </c>
       <c r="F14" s="3"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="29">
-        <v>40</v>
-      </c>
-      <c r="I14" s="22">
+      <c r="G14" s="18"/>
+      <c r="H14" s="25">
+        <v>40</v>
+      </c>
+      <c r="I14" s="18">
         <f t="shared" si="2"/>
         <v>122.672</v>
       </c>
@@ -1818,7 +1804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>43945</v>
       </c>
@@ -1831,11 +1817,11 @@
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="29">
-        <v>40</v>
-      </c>
-      <c r="I15" s="22">
+      <c r="G15" s="18"/>
+      <c r="H15" s="25">
+        <v>40</v>
+      </c>
+      <c r="I15" s="18">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
@@ -1848,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>43948</v>
       </c>
@@ -1861,19 +1847,19 @@
       <c r="D16" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="23">
         <v>78.036000000000001</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G16" s="22">
+      <c r="G16" s="18">
         <v>8.016</v>
       </c>
-      <c r="H16" s="29">
-        <v>40</v>
-      </c>
-      <c r="I16" s="22">
+      <c r="H16" s="25">
+        <v>40</v>
+      </c>
+      <c r="I16" s="18">
         <f t="shared" si="2"/>
         <v>126.05200000000001</v>
       </c>
@@ -1886,7 +1872,7 @@
         <v>24.050405040504053</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>43948</v>
       </c>
@@ -1899,11 +1885,11 @@
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="29">
-        <v>40</v>
-      </c>
-      <c r="I17" s="22">
+      <c r="G17" s="18"/>
+      <c r="H17" s="25">
+        <v>40</v>
+      </c>
+      <c r="I17" s="18">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
@@ -1916,7 +1902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>43949</v>
       </c>
@@ -1935,13 +1921,13 @@
       <c r="F18" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="22">
+      <c r="G18" s="18">
         <v>11.69</v>
       </c>
-      <c r="H18" s="29">
-        <v>40</v>
-      </c>
-      <c r="I18" s="22">
+      <c r="H18" s="25">
+        <v>40</v>
+      </c>
+      <c r="I18" s="18">
         <f>E18+G18+H18</f>
         <v>131.69</v>
       </c>
@@ -1954,7 +1940,7 @@
         <v>35.073507350735071</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>43949</v>
       </c>
@@ -1968,10 +1954,10 @@
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="29">
-        <v>40</v>
-      </c>
-      <c r="I19" s="22">
+      <c r="H19" s="25">
+        <v>40</v>
+      </c>
+      <c r="I19" s="18">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
@@ -1984,7 +1970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1992,10 +1978,10 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="7"/>
-      <c r="H20" s="29">
-        <v>40</v>
-      </c>
-      <c r="I20" s="22">
+      <c r="H20" s="25">
+        <v>40</v>
+      </c>
+      <c r="I20" s="18">
         <f>E20+G20+H20</f>
         <v>40</v>
       </c>
@@ -2008,35 +1994,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I21" s="24">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I21" s="20">
         <f>SUM(I10:I20)</f>
         <v>896.15200000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H23" s="25" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H23" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="I23" s="26">
+      <c r="I23" s="22">
         <f>I21</f>
         <v>896.15200000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H24" s="25" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H24" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="I24" s="26">
+      <c r="I24" s="22">
         <f>I23*18%</f>
         <v>161.30735999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="H25" s="25" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H25" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="I25" s="26">
+      <c r="I25" s="22">
         <f>I23+I24</f>
         <v>1057.4593600000001</v>
       </c>

</xml_diff>